<commit_message>
Remove Wong, add Estapa to flux comparison figure
</commit_message>
<xml_diff>
--- a/pocfluxes_fromKB_v2.xlsx
+++ b/pocfluxes_fromKB_v2.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vamaral/GoogleDrive/DOCS/Py_work/pyEXPORTS/invPOC_misc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vamaral/GoogleDrive/DOCS/Py_work/pyEXPORTS/invPOC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B20E059-BFC8-A244-A980-0DC7389F22BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC851D5C-4612-DF49-A335-AA9301BDAAFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26300" yWindow="460" windowWidth="25040" windowHeight="14000" xr2:uid="{FD536C54-43E7-9449-8341-BF955EBA5598}"/>
+    <workbookView xWindow="26940" yWindow="460" windowWidth="25040" windowHeight="14000" activeTab="1" xr2:uid="{FD536C54-43E7-9449-8341-BF955EBA5598}"/>
   </bookViews>
   <sheets>
-    <sheet name="to_df" sheetId="3" r:id="rId1"/>
+    <sheet name="thorium" sheetId="3" r:id="rId1"/>
+    <sheet name="traps" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>depth</t>
   </si>
@@ -55,6 +56,12 @@
   </si>
   <si>
     <t>msf_u</t>
+  </si>
+  <si>
+    <t>flux</t>
+  </si>
+  <si>
+    <t>flux_u</t>
   </si>
 </sst>
 </file>
@@ -408,7 +415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDAEBE9-9EC7-854E-AAFE-F4682E0CBD8C}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -670,4 +677,85 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD986AB6-763C-914C-B842-39E5FE775D91}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>1.3848625432886685</v>
+      </c>
+      <c r="C2">
+        <v>0.7719548047810465</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>150</v>
+      </c>
+      <c r="B3">
+        <v>1.0407822367945465</v>
+      </c>
+      <c r="C3">
+        <v>0.38784151665860167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>200</v>
+      </c>
+      <c r="B4">
+        <v>0.75568080420966999</v>
+      </c>
+      <c r="C4">
+        <v>0.23729528471901881</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>330</v>
+      </c>
+      <c r="B5">
+        <v>0.64319121464272433</v>
+      </c>
+      <c r="C5">
+        <v>0.28415347289088116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>500</v>
+      </c>
+      <c r="B6">
+        <v>0.85783057996062873</v>
+      </c>
+      <c r="C6">
+        <v>0.43077789507666842</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>